<commit_message>
Some minor spell changes& changed the name of `holy damage' to `celestial damage'
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/darkarts.xlsx
+++ b/CoreRulebook/Data/Spells/darkarts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HPRPG\CoreRulebook\Data\Spells\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B995AA2-369C-4612-AE3F-64C7776BE30B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8A707E-D3B0-47BB-85AF-AAA7B024F9FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="735" yWindow="645" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,10 +380,6 @@
     <t>confusangui</t>
   </si>
   <si>
-    <t xml:space="preserve">Use blood to draw warding runes onto an object or person. Erects a swirling red magical barrier with AC 10, plus 5 for every casting point over the difficulty. Barrier blocks all physical and magical damage and is immune to acid erosion, but is eroded by holy damage. 
-Each individual{\apos}s blood can only be used once for blood magic.  </t>
-  </si>
-  <si>
     <t>Create Thrall</t>
   </si>
   <si>
@@ -630,6 +626,10 @@
   </si>
   <si>
     <t>1 day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use blood to draw warding runes onto an object or person. Erects a swirling red magical barrier with AC 10, plus 5 for every casting point over the difficulty. Barrier blocks all physical and magical damage and is immune to acid erosion, but is eroded by celestial damage. 
+Each individual{\apos}s blood can only be used once for blood magic.  </t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1139,10 @@
   <dimension ref="A1:AME31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1540,10 +1540,10 @@
         <v>71</v>
       </c>
       <c r="I13" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="J13" s="11" t="s">
         <v>143</v>
-      </c>
-      <c r="J13" s="11" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
@@ -1616,7 +1616,7 @@
     </row>
     <row r="16" spans="1:11" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B16" s="7" t="s">
         <v>19</v>
@@ -1651,7 +1651,7 @@
         <v>88</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" s="10"/>
       <c r="F17" s="10">
@@ -1663,18 +1663,18 @@
       <c r="H17" s="12"/>
       <c r="I17" s="12"/>
       <c r="J17" s="11" t="s">
-        <v>89</v>
+        <v>152</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B18" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>52</v>
@@ -1693,21 +1693,21 @@
         <v>43</v>
       </c>
       <c r="J18" s="7" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="22.7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="8">
@@ -1719,28 +1719,28 @@
       <c r="H19" s="8"/>
       <c r="I19" s="8"/>
       <c r="J19" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K19" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>19</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="8" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G20" s="8">
         <v>4</v>
@@ -1748,21 +1748,21 @@
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
       <c r="J20" s="7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="50.65" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>103</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>104</v>
       </c>
       <c r="E21" s="8"/>
       <c r="F21" s="8">
@@ -1774,24 +1774,24 @@
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
       <c r="J21" s="7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F22" s="8">
         <v>0</v>
@@ -1802,24 +1802,24 @@
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
       <c r="J22" s="7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="41.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F23" s="8">
         <v>0</v>
@@ -1830,24 +1830,24 @@
       <c r="H23" s="8"/>
       <c r="I23" s="8"/>
       <c r="J23" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>117</v>
       </c>
       <c r="F24" s="1">
         <v>0</v>
@@ -1856,21 +1856,21 @@
         <v>5</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="60" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="F25" s="1">
         <v>3</v>
@@ -1879,27 +1879,27 @@
         <v>1</v>
       </c>
       <c r="J25" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>80</v>
@@ -1908,27 +1908,27 @@
         <v>3</v>
       </c>
       <c r="J26" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G27" s="1">
         <v>2</v>
@@ -1940,27 +1940,27 @@
         <v>43</v>
       </c>
       <c r="J27" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="K27" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="28" spans="1:11" ht="24" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>52</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F28" s="1">
         <v>0</v>
@@ -1969,18 +1969,18 @@
         <v>2</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="84" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F29" s="1">
         <v>0</v>
@@ -1989,50 +1989,50 @@
         <v>4</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="36" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>14</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G30" s="1">
         <v>2</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G31" s="1">
         <v>1</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Price changes+ new spells
</commit_message>
<xml_diff>
--- a/CoreRulebook/Data/Spells/darkarts.xlsx
+++ b/CoreRulebook/Data/Spells/darkarts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\HPRPG\CoreRulebook\Data\Spells\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8A707E-D3B0-47BB-85AF-AAA7B024F9FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94F36FA-FB04-4C08-B28C-2CD6F2A4A8AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="645" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3285" yWindow="3285" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -630,6 +630,30 @@
   <si>
     <t xml:space="preserve">Use blood to draw warding runes onto an object or person. Erects a swirling red magical barrier with AC 10, plus 5 for every casting point over the difficulty. Barrier blocks all physical and magical damage and is immune to acid erosion, but is eroded by celestial damage. 
 Each individual{\apos}s blood can only be used once for blood magic.  </t>
+  </si>
+  <si>
+    <t>Summoning Circle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By gathering together a group (only one of whom needs to be able to cast this spell), you create a special altar from which conjuration spells are especially powerful. The radius of this region is 2m, and whilst inside it, you gain a bonus to Conjuration casting checks equal to the number of people who created the summoning circle. </t>
+  </si>
+  <si>
+    <t>Blood Moon</t>
+  </si>
+  <si>
+    <t>Ritual (10 minutes)</t>
+  </si>
+  <si>
+    <t>Sky turns red</t>
+  </si>
+  <si>
+    <t>2 hours</t>
+  </si>
+  <si>
+    <t>When cast by a Master-level cast, this spell lasts for one week.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">By sacrificing an animal larger than a cat, you may use the inherent power of its blood to manipulate the power of the Sun and the Moon: the sky becomes overcast and takes on an unhealthy red glow. This blocks out the effects of the sun and the moon on Vampires, Werewolves, and other such creatures. Werewolves may still choose to undergo their transformation, but retain humanoid intelligence when doing so. </t>
   </si>
 </sst>
 </file>
@@ -1136,13 +1160,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AME31"/>
+  <dimension ref="A1:AME33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A17" sqref="A17"/>
-      <selection pane="bottomRight" activeCell="J18" sqref="J18"/>
+      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2035,6 +2059,49 @@
         <v>150</v>
       </c>
     </row>
+    <row r="32" spans="1:11" ht="36" x14ac:dyDescent="0.2">
+      <c r="A32" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="G32" s="1">
+        <v>4</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="48" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="G33" s="1">
+        <v>3</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>